<commit_message>
added two novel data
</commit_message>
<xml_diff>
--- a/工作簿1.xlsx
+++ b/工作簿1.xlsx
@@ -8,31 +8,37 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ErnestsExercises\Interesting\WordCounter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE7E037-D920-487D-A5B3-5B259BEC40E5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7926DB66-4B3F-432F-8208-336640E5DEBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E6D162C4-85F8-4240-B591-3FAB81AC097B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{E6D162C4-85F8-4240-B591-3FAB81AC097B}"/>
   </bookViews>
   <sheets>
     <sheet name="诗经" sheetId="13" r:id="rId1"/>
     <sheet name="唐诗三百首" sheetId="12" r:id="rId2"/>
     <sheet name="宋词三百首" sheetId="11" r:id="rId3"/>
-    <sheet name="三国演义" sheetId="9" r:id="rId4"/>
-    <sheet name="四世同堂" sheetId="8" r:id="rId5"/>
-    <sheet name="白鹿原" sheetId="1" r:id="rId6"/>
+    <sheet name="聊斋志异" sheetId="15" r:id="rId4"/>
+    <sheet name="红楼梦" sheetId="14" r:id="rId5"/>
+    <sheet name="三国演义" sheetId="9" r:id="rId6"/>
+    <sheet name="四世同堂" sheetId="8" r:id="rId7"/>
+    <sheet name="白鹿原" sheetId="1" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlchart.v1.0" hidden="1">诗经!$A$1:$A$20</definedName>
     <definedName name="_xlchart.v1.1" hidden="1">诗经!$B$1:$B$20</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">白鹿原!$A$1:$A$20</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">白鹿原!$B$1:$B$20</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">三国演义!$A$1:$A$20</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">三国演义!$B$1:$B$20</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">四世同堂!$A$1:$A$20</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">四世同堂!$B$1:$B$20</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">白鹿原!$A$1:$A$20</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">白鹿原!$B$1:$B$20</definedName>
     <definedName name="_xlchart.v1.2" hidden="1">唐诗三百首!$A$1:$A$20</definedName>
     <definedName name="_xlchart.v1.3" hidden="1">唐诗三百首!$B$1:$B$20</definedName>
     <definedName name="_xlchart.v1.4" hidden="1">宋词三百首!$A$1:$A$20</definedName>
     <definedName name="_xlchart.v1.5" hidden="1">宋词三百首!$B$1:$B$20</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">三国演义!$A$1:$A$20</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">三国演义!$B$1:$B$20</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">四世同堂!$A$1:$A$20</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">四世同堂!$B$1:$B$20</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">聊斋志异!$A$1:$A$20</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">聊斋志异!$B$1:$B$20</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">红楼梦!$A$1:$A$20</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">红楼梦!$B$1:$B$20</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -52,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="79">
   <si>
     <t>的</t>
   </si>
@@ -265,6 +271,30 @@
   </si>
   <si>
     <t>没</t>
+  </si>
+  <si>
+    <t>道</t>
+  </si>
+  <si>
+    <t>这</t>
+  </si>
+  <si>
+    <t>儿</t>
+  </si>
+  <si>
+    <t>也</t>
+  </si>
+  <si>
+    <t>玉</t>
+  </si>
+  <si>
+    <t>宝</t>
+  </si>
+  <si>
+    <t>女</t>
+  </si>
+  <si>
+    <t>者</t>
   </si>
 </sst>
 </file>
@@ -659,7 +689,7 @@
                 <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
                 <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
               </a:rPr>
-              <a:t>三国演义</a:t>
+              <a:t>聊斋志异</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN" sz="1600" b="1" i="0" u="none" strike="noStrike" cap="all" baseline="0">
@@ -777,7 +807,7 @@
                 <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
                 <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
               </a:rPr>
-              <a:t>四世同堂</a:t>
+              <a:t>红楼梦</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" altLang="zh-CN" sz="1600" b="1" i="0" u="none" strike="noStrike" cap="all" baseline="0">
@@ -858,6 +888,242 @@
       </cx:strDim>
       <cx:numDim type="size">
         <cx:f>_xlchart.v1.11</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1600" b="1" i="0" u="none" strike="noStrike" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              </a:rPr>
+              <a:t>《</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              </a:rPr>
+              <a:t>三国演义</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1600" b="1" i="0" u="none" strike="noStrike" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              </a:rPr>
+              <a:t>》</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1050" b="0" i="0" u="none" strike="noStrike" cap="all" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="treemap" uniqueId="{FA9106F9-4E4A-4712-806B-0D052D6CC775}">
+          <cx:dataLabels pos="ctr">
+            <cx:txPr>
+              <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr sz="1800">
+                    <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                    <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                    <a:cs typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="window" lastClr="FFFFFF"/>
+                  </a:solidFill>
+                  <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                  <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                </a:endParaRPr>
+              </a:p>
+            </cx:txPr>
+            <cx:visibility seriesName="0" categoryName="1" value="1"/>
+            <cx:separator> </cx:separator>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:parentLabelLayout val="overlapping"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+  </cx:chart>
+  <cx:spPr>
+    <a:solidFill>
+      <a:srgbClr val="F0EFE4"/>
+    </a:solidFill>
+  </cx:spPr>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx7.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.12</cx:f>
+      </cx:strDim>
+      <cx:numDim type="size">
+        <cx:f>_xlchart.v1.13</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr" rtl="0">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1600" b="1" i="0" u="none" strike="noStrike" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              </a:rPr>
+              <a:t>《</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="zh-CN" altLang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              </a:rPr>
+              <a:t>四世同堂</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1600" b="1" i="0" u="none" strike="noStrike" cap="all" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+                <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              </a:rPr>
+              <a:t>》</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" altLang="zh-CN" sz="1050" b="0" i="0" u="none" strike="noStrike" cap="all" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+              <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+            </a:endParaRPr>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="treemap" uniqueId="{FA9106F9-4E4A-4712-806B-0D052D6CC775}">
+          <cx:dataLabels pos="ctr">
+            <cx:txPr>
+              <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr algn="ctr" rtl="0">
+                  <a:defRPr sz="1800">
+                    <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                    <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                    <a:cs typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="window" lastClr="FFFFFF"/>
+                  </a:solidFill>
+                  <a:latin typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                  <a:ea typeface="微软雅黑" panose="020B0503020204020204" pitchFamily="34" charset="-122"/>
+                </a:endParaRPr>
+              </a:p>
+            </cx:txPr>
+            <cx:visibility seriesName="0" categoryName="1" value="1"/>
+            <cx:separator> </cx:separator>
+          </cx:dataLabels>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:parentLabelLayout val="overlapping"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+    </cx:plotArea>
+  </cx:chart>
+  <cx:spPr>
+    <a:solidFill>
+      <a:srgbClr val="F0EFE4"/>
+    </a:solidFill>
+  </cx:spPr>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx8.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.14</cx:f>
+      </cx:strDim>
+      <cx:numDim type="size">
+        <cx:f>_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1207,6 +1473,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="416">
   <cs:axisTitle>
@@ -3763,6 +4109,1028 @@
 </file>
 
 <file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="416">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1">
+          <a:lumMod val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" b="1"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" cap="all"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="416">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1">
+          <a:lumMod val="65000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" b="1"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" cap="all"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="416">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -4532,6 +5900,172 @@
       <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="图表 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{43ADC2AC-6DB7-4750-9E72-3E666A37FEF9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3413760" y="457200"/>
+              <a:ext cx="7444740" cy="3307080"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+                <a:t>此图表在您的 Excel 版本中不可用。
+编辑此形状或将此工作簿转换为其他文件格式将永久破坏图表。</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="图表 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34D4F17B-53A7-4596-9998-06EF517A2202}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3413760" y="457200"/>
+              <a:ext cx="7444740" cy="3307080"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="zh-CN" altLang="en-US" sz="1100"/>
+                <a:t>此图表在您的 Excel 版本中不可用。
+编辑此形状或将此工作簿转换为其他文件格式将永久破坏图表。</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>365760</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>381000</xdr:colOff>
       <xdr:row>23</xdr:row>
@@ -4605,7 +6139,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -4688,7 +6222,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5070,7 +6604,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE7F270-B0A4-4AF1-92ED-2C01417DE2CA}">
   <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R13" sqref="R13"/>
     </sheetView>
   </sheetViews>
@@ -5598,6 +7132,360 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1F9E659-73E2-4BE6-BA10-FB3C082BFEDA}">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1">
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>1.74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3">
+        <v>1.45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>1.34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5">
+        <v>1.23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6">
+        <v>1.1299999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>41</v>
+      </c>
+      <c r="B13">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14">
+        <v>0.56000000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20">
+        <v>0.5</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{995D15EA-2D89-476D-98D7-00DC785B3BE8}">
+  <dimension ref="A1:B20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T15" sqref="T15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <v>2.93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2.17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3">
+        <v>2.02</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1.62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>1.38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>1.33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B11">
+        <v>1.06</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>0.98</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B14">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>65</v>
+      </c>
+      <c r="B17">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20">
+        <v>0.81</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7502153-C6A7-43C1-9595-2400FBAA6FA4}">
   <dimension ref="A1:B20"/>
   <sheetViews>
@@ -5774,7 +7662,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC34AF44-8411-474C-A344-E32803CEC508}">
   <dimension ref="A1:B20"/>
   <sheetViews>
@@ -5951,7 +7839,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C387CC-01EB-4349-8B57-C6851B8AA616}">
   <dimension ref="A1:B20"/>
   <sheetViews>

</xml_diff>